<commit_message>
Added titles to dashboard figures
</commit_message>
<xml_diff>
--- a/group_comparison/five_cohort_sample_comparison_dashboard_custom_colors.xlsx
+++ b/group_comparison/five_cohort_sample_comparison_dashboard_custom_colors.xlsx
@@ -198,7 +198,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="10715625" cy="8239125"/>
+    <ext cx="10715625" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -228,7 +228,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="10772775" cy="8534400"/>
+    <ext cx="10772775" cy="8934450"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -258,7 +258,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6162675"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -288,7 +288,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8029575" cy="6162675"/>
+    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -318,7 +318,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8029575" cy="6162675"/>
+    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -348,7 +348,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6162675"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -378,7 +378,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6162675"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -408,7 +408,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8029575" cy="6162675"/>
+    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -438,7 +438,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8029575" cy="6162675"/>
+    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -468,7 +468,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6162675"/>
+    <ext cx="8277225" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -498,7 +498,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6162675"/>
+    <ext cx="8277225" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -528,7 +528,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="10944225" cy="8239125"/>
+    <ext cx="10944225" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -558,7 +558,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8382000" cy="6162675"/>
+    <ext cx="8382000" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -588,7 +588,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6162675"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -618,7 +618,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6162675"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -648,7 +648,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6162675"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -678,7 +678,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8591550" cy="6686550"/>
+    <ext cx="8591550" cy="6991350"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -708,7 +708,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8601075" cy="6686550"/>
+    <ext cx="8601075" cy="6991350"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -738,7 +738,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6686550"/>
+    <ext cx="8153400" cy="6991350"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -768,7 +768,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="11020425" cy="8239125"/>
+    <ext cx="11020425" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -798,7 +798,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="11220450" cy="8239125"/>
+    <ext cx="11220450" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -828,7 +828,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="10972800" cy="8239125"/>
+    <ext cx="10972800" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -858,7 +858,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="10944225" cy="8239125"/>
+    <ext cx="10944225" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -888,7 +888,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="10944225" cy="8239125"/>
+    <ext cx="10944225" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -918,7 +918,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="11220450" cy="8239125"/>
+    <ext cx="11220450" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -948,7 +948,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="11277600" cy="8239125"/>
+    <ext cx="11277600" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>

</xml_diff>

<commit_message>
Reran group comparison tutorial with newest dashboard generator
</commit_message>
<xml_diff>
--- a/group_comparison/five_cohort_sample_comparison_dashboard_custom_colors.xlsx
+++ b/group_comparison/five_cohort_sample_comparison_dashboard_custom_colors.xlsx
@@ -53,23 +53,24 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Start active pores vs. AUC" sheetId="45" state="visible" r:id="rId45"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg active pores vs. data" sheetId="46" state="visible" r:id="rId46"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pore AUC vs. data" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg pore occup. vs. data" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transloc. speed vs. Q score" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data output vs. Q score" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Start. pores vs. Q score" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pore AUC vs. Q score" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Passed bases vs. Q score" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="54" state="visible" r:id="rId54"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="55" state="visible" r:id="rId55"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="56" state="visible" r:id="rId56"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="57" state="visible" r:id="rId57"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore diff. vs. active pore AUC" sheetId="58" state="visible" r:id="rId58"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore occup. vs. pore diff." sheetId="59" state="visible" r:id="rId59"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="60" state="visible" r:id="rId60"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="61" state="visible" r:id="rId61"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="62" state="visible" r:id="rId62"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="63" state="visible" r:id="rId63"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore AUC vs. read count" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg pore occup. vs. data" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transloc. speed vs. Q score" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data output vs. Q score" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Start. pores vs. Q score" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Active pore AUC vs. Q score" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Passed bases vs. Q score" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. starting active pores" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pqc vs. pore difference" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore diff. vs. active pore AUC" sheetId="59" state="visible" r:id="rId59"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore occup. vs. pore diff." sheetId="60" state="visible" r:id="rId60"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="65" state="visible" r:id="rId65"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1001,6 +1002,36 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
+    <ext cx="8029575" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing34.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
     <ext cx="8162925" cy="6457950"/>
     <pic>
       <nvPicPr>
@@ -1022,7 +1053,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1052,7 +1083,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1082,7 +1113,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing37.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1092,36 +1123,6 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="8143875" cy="6457950"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing37.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1181,7 +1182,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8277225" cy="6457950"/>
+    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1271,6 +1272,36 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
+    <ext cx="8277225" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing42.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
     <ext cx="8382000" cy="6457950"/>
     <pic>
       <nvPicPr>
@@ -1292,7 +1323,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing43.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1322,7 +1353,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing44.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1352,7 +1383,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing45.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1362,36 +1393,6 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="8420100" cy="6457950"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing45.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1451,6 +1452,36 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
+    <ext cx="8153400" cy="6457950"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing48.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
     <ext cx="8591550" cy="6991350"/>
     <pic>
       <nvPicPr>
@@ -1472,7 +1503,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing49.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1502,7 +1533,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1511,7 +1542,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6991350"/>
+    <ext cx="11220450" cy="8648700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1532,7 +1563,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing50.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1541,7 +1572,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="11220450" cy="8648700"/>
+    <ext cx="8153400" cy="6991350"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -2043,7 +2074,7 @@
         <v>25.39</v>
       </c>
       <c r="G2" t="n">
-        <v>21.73</v>
+        <v>25.4</v>
       </c>
       <c r="H2" t="n">
         <v>2.923</v>
@@ -2071,7 +2102,7 @@
         <v>69.072</v>
       </c>
       <c r="G3" t="n">
-        <v>55.478</v>
+        <v>58.149</v>
       </c>
       <c r="H3" t="n">
         <v>18.311</v>
@@ -2099,7 +2130,7 @@
         <v>7.524</v>
       </c>
       <c r="G4" t="n">
-        <v>6.53</v>
+        <v>7.862</v>
       </c>
       <c r="H4" t="n">
         <v>1.819</v>
@@ -2127,7 +2158,7 @@
         <v>7136.5</v>
       </c>
       <c r="G5" t="n">
-        <v>6977</v>
+        <v>8849</v>
       </c>
       <c r="H5" t="n">
         <v>747.265</v>
@@ -2155,7 +2186,7 @@
         <v>2386.724</v>
       </c>
       <c r="G6" t="n">
-        <v>2404.043</v>
+        <v>2219.234</v>
       </c>
       <c r="H6" t="n">
         <v>592.8579999999999</v>
@@ -2323,7 +2354,7 @@
         <v>110974</v>
       </c>
       <c r="G12" t="n">
-        <v>110586</v>
+        <v>104304</v>
       </c>
       <c r="H12" t="n">
         <v>26638.35</v>
@@ -2351,7 +2382,7 @@
         <v>96.622</v>
       </c>
       <c r="G13" t="n">
-        <v>94.41800000000001</v>
+        <v>97.113</v>
       </c>
       <c r="H13" t="n">
         <v>1.948</v>
@@ -2379,7 +2410,7 @@
         <v>94.965</v>
       </c>
       <c r="G14" t="n">
-        <v>83.11799999999999</v>
+        <v>92.70099999999999</v>
       </c>
       <c r="H14" t="n">
         <v>3.405</v>
@@ -2662,7 +2693,7 @@
         <v>24.55</v>
       </c>
       <c r="G2" t="n">
-        <v>24.68</v>
+        <v>20.56</v>
       </c>
       <c r="H2" t="n">
         <v>3.127</v>
@@ -2690,7 +2721,7 @@
         <v>88.035</v>
       </c>
       <c r="G3" t="n">
-        <v>88.035</v>
+        <v>125.613</v>
       </c>
       <c r="H3" t="n">
         <v>35.772</v>
@@ -2718,7 +2749,7 @@
         <v>6.619</v>
       </c>
       <c r="G4" t="n">
-        <v>10.406</v>
+        <v>9.33</v>
       </c>
       <c r="H4" t="n">
         <v>3.241</v>
@@ -2746,7 +2777,7 @@
         <v>6210</v>
       </c>
       <c r="G5" t="n">
-        <v>6077</v>
+        <v>5488</v>
       </c>
       <c r="H5" t="n">
         <v>1389.558</v>
@@ -2774,7 +2805,7 @@
         <v>3312.273</v>
       </c>
       <c r="G6" t="n">
-        <v>2964.6</v>
+        <v>3921.227</v>
       </c>
       <c r="H6" t="n">
         <v>997.537</v>
@@ -2942,7 +2973,7 @@
         <v>133407</v>
       </c>
       <c r="G12" t="n">
-        <v>133407</v>
+        <v>172534</v>
       </c>
       <c r="H12" t="n">
         <v>48910.689</v>
@@ -2970,7 +3001,7 @@
         <v>95.033</v>
       </c>
       <c r="G13" t="n">
-        <v>93.601</v>
+        <v>95.985</v>
       </c>
       <c r="H13" t="n">
         <v>9.019</v>
@@ -2998,7 +3029,7 @@
         <v>94.57899999999999</v>
       </c>
       <c r="G14" t="n">
-        <v>93.087</v>
+        <v>96.98099999999999</v>
       </c>
       <c r="H14" t="n">
         <v>15.708</v>
@@ -3082,7 +3113,7 @@
         <v>398.772</v>
       </c>
       <c r="G17" t="n">
-        <v>399.133</v>
+        <v>396.319</v>
       </c>
       <c r="H17" t="n">
         <v>3.772</v>
@@ -3110,7 +3141,7 @@
         <v>390.99</v>
       </c>
       <c r="G18" t="n">
-        <v>395.786</v>
+        <v>396.553</v>
       </c>
       <c r="H18" t="n">
         <v>6.128</v>
@@ -3138,7 +3169,7 @@
         <v>12.017</v>
       </c>
       <c r="G19" t="n">
-        <v>6.037</v>
+        <v>12.079</v>
       </c>
       <c r="H19" t="n">
         <v>2.459</v>
@@ -3166,7 +3197,7 @@
         <v>11.568</v>
       </c>
       <c r="G20" t="n">
-        <v>7.973</v>
+        <v>12.011</v>
       </c>
       <c r="H20" t="n">
         <v>2.035</v>
@@ -3194,7 +3225,7 @@
         <v>79.15900000000001</v>
       </c>
       <c r="G21" t="n">
-        <v>77.17700000000001</v>
+        <v>111.062</v>
       </c>
       <c r="H21" t="n">
         <v>34.006</v>
@@ -3222,7 +3253,7 @@
         <v>8.286</v>
       </c>
       <c r="G22" t="n">
-        <v>10.193</v>
+        <v>14.299</v>
       </c>
       <c r="H22" t="n">
         <v>3.628</v>
@@ -3250,7 +3281,7 @@
         <v>89.38500000000001</v>
       </c>
       <c r="G23" t="n">
-        <v>88.334</v>
+        <v>88.59399999999999</v>
       </c>
       <c r="H23" t="n">
         <v>9.083</v>
@@ -3330,7 +3361,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Top up</t>
+          <t>Run type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -3390,7 +3421,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3410,7 +3441,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3430,7 +3461,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3450,7 +3481,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3470,7 +3501,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3510,7 +3541,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3530,7 +3561,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3570,7 +3601,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3590,7 +3621,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -3610,7 +3641,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -3630,7 +3661,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -3650,7 +3681,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -3670,7 +3701,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -3690,7 +3721,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -3710,7 +3741,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -4213,7 +4244,7 @@
         <v>85.944</v>
       </c>
       <c r="G3" t="n">
-        <v>125.76</v>
+        <v>43.103</v>
       </c>
       <c r="H3" t="n">
         <v>47.286</v>
@@ -4241,7 +4272,7 @@
         <v>5.601</v>
       </c>
       <c r="G4" t="n">
-        <v>7.697</v>
+        <v>3.662</v>
       </c>
       <c r="H4" t="n">
         <v>3.139</v>
@@ -4269,7 +4300,7 @@
         <v>6621.5</v>
       </c>
       <c r="G5" t="n">
-        <v>6810</v>
+        <v>3442</v>
       </c>
       <c r="H5" t="n">
         <v>1525.017</v>
@@ -4297,7 +4328,7 @@
         <v>2891.69</v>
       </c>
       <c r="G6" t="n">
-        <v>3050.593</v>
+        <v>1386.733</v>
       </c>
       <c r="H6" t="n">
         <v>1141.989</v>
@@ -4465,7 +4496,7 @@
         <v>130191.5</v>
       </c>
       <c r="G12" t="n">
-        <v>179985</v>
+        <v>62403</v>
       </c>
       <c r="H12" t="n">
         <v>67529.807</v>
@@ -4493,7 +4524,7 @@
         <v>96.224</v>
       </c>
       <c r="G13" t="n">
-        <v>96.575</v>
+        <v>94.172</v>
       </c>
       <c r="H13" t="n">
         <v>10.066</v>
@@ -4521,7 +4552,7 @@
         <v>92.86</v>
       </c>
       <c r="G14" t="n">
-        <v>95.042</v>
+        <v>87.52200000000001</v>
       </c>
       <c r="H14" t="n">
         <v>19.708</v>
@@ -4605,7 +4636,7 @@
         <v>397.696</v>
       </c>
       <c r="G17" t="n">
-        <v>395.457</v>
+        <v>396.964</v>
       </c>
       <c r="H17" t="n">
         <v>2.456</v>
@@ -4633,7 +4664,7 @@
         <v>389.84</v>
       </c>
       <c r="G18" t="n">
-        <v>388.434</v>
+        <v>393.362</v>
       </c>
       <c r="H18" t="n">
         <v>11.951</v>
@@ -4661,7 +4692,7 @@
         <v>12.692</v>
       </c>
       <c r="G19" t="n">
-        <v>12.648</v>
+        <v>10.22</v>
       </c>
       <c r="H19" t="n">
         <v>1.517</v>
@@ -4689,7 +4720,7 @@
         <v>12.16</v>
       </c>
       <c r="G20" t="n">
-        <v>12.401</v>
+        <v>8.981999999999999</v>
       </c>
       <c r="H20" t="n">
         <v>1.882</v>
@@ -4717,7 +4748,7 @@
         <v>78.92700000000001</v>
       </c>
       <c r="G21" t="n">
-        <v>115.967</v>
+        <v>35.812</v>
       </c>
       <c r="H21" t="n">
         <v>45.375</v>
@@ -4745,7 +4776,7 @@
         <v>7.288</v>
       </c>
       <c r="G22" t="n">
-        <v>10.632</v>
+        <v>6.955</v>
       </c>
       <c r="H22" t="n">
         <v>3.401</v>
@@ -4773,7 +4804,7 @@
         <v>92.38800000000001</v>
       </c>
       <c r="G23" t="n">
-        <v>91.602</v>
+        <v>83.73699999999999</v>
       </c>
       <c r="H23" t="n">
         <v>13.432</v>
@@ -4861,7 +4892,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Top up</t>
+          <t>Run type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -4881,7 +4912,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -4901,7 +4932,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -4921,7 +4952,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -4941,7 +4972,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -4961,7 +4992,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -4981,7 +5012,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -5001,7 +5032,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -5021,7 +5052,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -5041,7 +5072,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -5061,7 +5092,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -5141,7 +5172,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -5161,7 +5192,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -5181,7 +5212,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -5201,7 +5232,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -5241,7 +5272,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -5261,7 +5292,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -5761,7 +5792,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Top up</t>
+          <t>Run type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -5781,7 +5812,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -5801,7 +5832,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -5821,7 +5852,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -5841,7 +5872,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -5861,7 +5892,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -5881,7 +5912,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -5901,7 +5932,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -5921,7 +5952,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -5941,7 +5972,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -5961,7 +5992,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -5981,7 +6012,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -6001,7 +6032,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -6021,7 +6052,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -6041,7 +6072,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -6061,7 +6092,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -6081,7 +6112,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -6101,7 +6132,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -6121,7 +6152,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -6141,7 +6172,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -6161,7 +6192,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -6998,7 +7029,7 @@
         <v>31.11</v>
       </c>
       <c r="G2" t="n">
-        <v>36.97</v>
+        <v>32.16</v>
       </c>
       <c r="H2" t="n">
         <v>4.293</v>
@@ -7026,7 +7057,7 @@
         <v>65.161</v>
       </c>
       <c r="G3" t="n">
-        <v>5.955</v>
+        <v>78.488</v>
       </c>
       <c r="H3" t="n">
         <v>29.728</v>
@@ -7054,7 +7085,7 @@
         <v>3.571</v>
       </c>
       <c r="G4" t="n">
-        <v>0.267</v>
+        <v>3.964</v>
       </c>
       <c r="H4" t="n">
         <v>1.616</v>
@@ -7082,7 +7113,7 @@
         <v>7144</v>
       </c>
       <c r="G5" t="n">
-        <v>9018</v>
+        <v>7431</v>
       </c>
       <c r="H5" t="n">
         <v>1214.904</v>
@@ -7110,7 +7141,7 @@
         <v>2611.696</v>
       </c>
       <c r="G6" t="n">
-        <v>8631.5</v>
+        <v>2546.167</v>
       </c>
       <c r="H6" t="n">
         <v>1637.322</v>
@@ -7278,7 +7309,7 @@
         <v>103654</v>
       </c>
       <c r="G12" t="n">
-        <v>17263</v>
+        <v>122216</v>
       </c>
       <c r="H12" t="n">
         <v>46435.422</v>
@@ -7306,7 +7337,7 @@
         <v>93.083</v>
       </c>
       <c r="G13" t="n">
-        <v>90.527</v>
+        <v>90.626</v>
       </c>
       <c r="H13" t="n">
         <v>4.248</v>
@@ -7334,7 +7365,7 @@
         <v>92.515</v>
       </c>
       <c r="G14" t="n">
-        <v>97.279</v>
+        <v>90.827</v>
       </c>
       <c r="H14" t="n">
         <v>4.107</v>
@@ -7381,6 +7412,9 @@
       <c r="F17" t="n">
         <v>398.682</v>
       </c>
+      <c r="G17" t="n">
+        <v>397.981</v>
+      </c>
       <c r="H17" t="n">
         <v>0.702</v>
       </c>
@@ -7406,6 +7440,9 @@
       <c r="F18" t="n">
         <v>394.477</v>
       </c>
+      <c r="G18" t="n">
+        <v>396.092</v>
+      </c>
       <c r="H18" t="n">
         <v>1.614</v>
       </c>
@@ -7431,6 +7468,9 @@
       <c r="F19" t="n">
         <v>11.822</v>
       </c>
+      <c r="G19" t="n">
+        <v>11.968</v>
+      </c>
       <c r="H19" t="n">
         <v>0.146</v>
       </c>
@@ -7455,6 +7495,9 @@
       </c>
       <c r="F20" t="n">
         <v>11.626</v>
+      </c>
+      <c r="G20" t="n">
+        <v>11.645</v>
       </c>
       <c r="H20" t="n">
         <v>0.019</v>
@@ -7818,7 +7861,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Top up</t>
+          <t>Run type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -7838,7 +7881,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -7858,7 +7901,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -7878,7 +7921,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -7898,7 +7941,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -7918,7 +7961,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -7938,7 +7981,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -7958,7 +8001,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -7978,7 +8021,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -7998,7 +8041,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -8018,7 +8061,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -8038,7 +8081,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -8058,7 +8101,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -8078,7 +8121,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -8138,7 +8181,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -8158,7 +8201,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -8178,7 +8221,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -8198,7 +8241,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -8880,6 +8923,25 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -8958,7 +9020,7 @@
         <v>24.78</v>
       </c>
       <c r="G2" t="n">
-        <v>24.36</v>
+        <v>27.57</v>
       </c>
       <c r="H2" t="n">
         <v>2.672</v>
@@ -8986,7 +9048,7 @@
         <v>85.447</v>
       </c>
       <c r="G3" t="n">
-        <v>109.059</v>
+        <v>88.35899999999999</v>
       </c>
       <c r="H3" t="n">
         <v>27.728</v>
@@ -9014,7 +9076,7 @@
         <v>4.484</v>
       </c>
       <c r="G4" t="n">
-        <v>5.859</v>
+        <v>4.452</v>
       </c>
       <c r="H4" t="n">
         <v>1.556</v>
@@ -9042,7 +9104,7 @@
         <v>6450</v>
       </c>
       <c r="G5" t="n">
-        <v>5979</v>
+        <v>7050</v>
       </c>
       <c r="H5" t="n">
         <v>947.67</v>
@@ -9070,7 +9132,7 @@
         <v>2735.133</v>
       </c>
       <c r="G6" t="n">
-        <v>3409.378</v>
+        <v>2927.558</v>
       </c>
       <c r="H6" t="n">
         <v>919.135</v>
@@ -9238,7 +9300,7 @@
         <v>123081</v>
       </c>
       <c r="G12" t="n">
-        <v>153422</v>
+        <v>125885</v>
       </c>
       <c r="H12" t="n">
         <v>39161.387</v>
@@ -9266,7 +9328,7 @@
         <v>95.703</v>
       </c>
       <c r="G13" t="n">
-        <v>97.961</v>
+        <v>92.786</v>
       </c>
       <c r="H13" t="n">
         <v>4.413</v>
@@ -9294,7 +9356,7 @@
         <v>92.98099999999999</v>
       </c>
       <c r="G14" t="n">
-        <v>97.797</v>
+        <v>86.126</v>
       </c>
       <c r="H14" t="n">
         <v>13.461</v>
@@ -9350,7 +9412,7 @@
         <v>5.85</v>
       </c>
       <c r="G16" t="n">
-        <v>5.85</v>
+        <v>5.55</v>
       </c>
       <c r="H16" t="n">
         <v>0.851</v>
@@ -9378,7 +9440,7 @@
         <v>398.219</v>
       </c>
       <c r="G17" t="n">
-        <v>404.656</v>
+        <v>399.407</v>
       </c>
       <c r="H17" t="n">
         <v>4.894</v>
@@ -9406,7 +9468,7 @@
         <v>386.689</v>
       </c>
       <c r="G18" t="n">
-        <v>391.317</v>
+        <v>373.87</v>
       </c>
       <c r="H18" t="n">
         <v>8.941000000000001</v>
@@ -9434,7 +9496,7 @@
         <v>12.226</v>
       </c>
       <c r="G19" t="n">
-        <v>13.281</v>
+        <v>12.226</v>
       </c>
       <c r="H19" t="n">
         <v>0.931</v>
@@ -9462,7 +9524,7 @@
         <v>11.375</v>
       </c>
       <c r="G20" t="n">
-        <v>13.054</v>
+        <v>10.96</v>
       </c>
       <c r="H20" t="n">
         <v>1.72</v>
@@ -9490,7 +9552,7 @@
         <v>79.084</v>
       </c>
       <c r="G21" t="n">
-        <v>99.062</v>
+        <v>82.063</v>
       </c>
       <c r="H21" t="n">
         <v>28.539</v>
@@ -9518,7 +9580,7 @@
         <v>7.854</v>
       </c>
       <c r="G22" t="n">
-        <v>10.478</v>
+        <v>7.512</v>
       </c>
       <c r="H22" t="n">
         <v>3.443</v>
@@ -9546,7 +9608,7 @@
         <v>90.51600000000001</v>
       </c>
       <c r="G23" t="n">
-        <v>90.435</v>
+        <v>91.614</v>
       </c>
       <c r="H23" t="n">
         <v>8.256</v>
@@ -9626,7 +9688,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Top up</t>
+          <t>Run type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -9746,7 +9808,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -9766,7 +9828,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -9786,7 +9848,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -9806,7 +9868,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -9826,7 +9888,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -9846,7 +9908,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -9866,7 +9928,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -9886,7 +9948,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -9906,7 +9968,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -9926,7 +9988,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -9946,7 +10008,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -9966,7 +10028,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -9986,7 +10048,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -10006,7 +10068,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Initial run</t>
+          <t>Standard run</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">

</xml_diff>

<commit_message>
Reran tutorials reflecting changes in reconnection identification
</commit_message>
<xml_diff>
--- a/group_comparison/five_cohort_sample_comparison_dashboard_custom_colors.xlsx
+++ b/group_comparison/five_cohort_sample_comparison_dashboard_custom_colors.xlsx
@@ -65,12 +65,13 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore vs. time difference" sheetId="57" state="visible" r:id="rId57"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference vs. run output" sheetId="58" state="visible" r:id="rId58"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore diff. vs. active pore AUC" sheetId="59" state="visible" r:id="rId59"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore occup. vs. pore diff." sheetId="60" state="visible" r:id="rId60"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="61" state="visible" r:id="rId61"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="62" state="visible" r:id="rId62"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="63" state="visible" r:id="rId63"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="64" state="visible" r:id="rId64"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore diff. vs. Q score" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore occup. vs. pore diff." sheetId="61" state="visible" r:id="rId61"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output pore diff" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N50 output starting pores" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Platform QC pores over time" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pore difference over time" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Run output over time" sheetId="66" state="visible" r:id="rId66"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1392,7 +1393,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8420100" cy="6457950"/>
+    <ext cx="8029575" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1422,7 +1423,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8153400" cy="6457950"/>
+    <ext cx="8420100" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1482,7 +1483,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8591550" cy="6991350"/>
+    <ext cx="8153400" cy="6457950"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1512,7 +1513,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8601075" cy="6991350"/>
+    <ext cx="8591550" cy="6991350"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -1564,6 +1565,36 @@
 </file>
 
 <file path=xl/drawings/drawing50.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8601075" cy="6991350"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing51.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -8942,6 +8973,25 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>